<commit_message>
added crustacea to the representativeness sheet
Former-commit-id: e7c0b60df299d8df8293833fe8af685ec4a759c7
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/spp_gp_representativeness.xlsx
+++ b/_raw_data/xlsx/spp_gp_representativeness.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="460" windowWidth="20500" windowHeight="13480" tabRatio="500"/>
+    <workbookView xWindow="2680" yWindow="4500" windowWidth="20500" windowHeight="13480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Casey O'Hara</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>from Claudia Arango re: crustacea_arthropods
+all species listed except N australe represent Class Malacostraca in Subphylum Crustacea</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="representativeness_blank.csv" type="6" refreshedVersion="0" background="1" saveData="1">
@@ -35,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="308">
   <si>
     <t>turbo militaris</t>
   </si>
@@ -880,9 +904,6 @@
     <t>class</t>
   </si>
   <si>
-    <t>comments/notes ORDER</t>
-  </si>
-  <si>
     <t>Holothuriida</t>
   </si>
   <si>
@@ -935,13 +956,40 @@
   </si>
   <si>
     <t>Species</t>
+  </si>
+  <si>
+    <t>hydrothermal crabs</t>
+  </si>
+  <si>
+    <t>soldier crabs</t>
+  </si>
+  <si>
+    <t>represents  Class Pycnogonida in subphylum Chelicerata --Not in Crustacea</t>
+  </si>
+  <si>
+    <t>general morphology, habitats and  life traits are representative at family level for all species listed except Palaemonidae, a large diverse family of &gt;1k+ spp.</t>
+  </si>
+  <si>
+    <t>king crabs</t>
+  </si>
+  <si>
+    <t>mud crabs</t>
+  </si>
+  <si>
+    <t>coral crabs</t>
+  </si>
+  <si>
+    <t>all species listed except N australe represent Class Malacostraca in Subphylum Crustacea</t>
+  </si>
+  <si>
+    <t>comments/notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -955,6 +1003,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -974,14 +1052,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1322,12 +1408,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E269"/>
+  <dimension ref="A1:F269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B271" sqref="B271"/>
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1339,7 +1425,7 @@
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>275</v>
       </c>
@@ -1350,13 +1436,13 @@
         <v>273</v>
       </c>
       <c r="D1" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="E1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
+    <row r="2" spans="1:6" hidden="1">
       <c r="A2" t="s">
         <v>272</v>
       </c>
@@ -1370,7 +1456,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>264</v>
       </c>
@@ -1378,13 +1464,16 @@
         <v>270</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>278</v>
+      </c>
+      <c r="D3" t="s">
+        <v>299</v>
       </c>
       <c r="E3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>264</v>
       </c>
@@ -1392,13 +1481,16 @@
         <v>269</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>278</v>
+      </c>
+      <c r="D4" t="s">
+        <v>300</v>
       </c>
       <c r="E4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>264</v>
       </c>
@@ -1406,13 +1498,19 @@
         <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>278</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>301</v>
       </c>
       <c r="E5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1">
+      <c r="F5" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="70">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -1420,13 +1518,16 @@
         <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>274</v>
+        <v>277</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="E6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>264</v>
       </c>
@@ -1434,10 +1535,13 @@
         <v>266</v>
       </c>
       <c r="C7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" hidden="1">
+        <v>278</v>
+      </c>
+      <c r="D7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>264</v>
       </c>
@@ -1445,10 +1549,13 @@
         <v>265</v>
       </c>
       <c r="C8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1">
+        <v>278</v>
+      </c>
+      <c r="D8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>264</v>
       </c>
@@ -1456,10 +1563,13 @@
         <v>263</v>
       </c>
       <c r="C9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1">
+        <v>278</v>
+      </c>
+      <c r="D9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -1470,10 +1580,10 @@
         <v>279</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -1484,10 +1594,10 @@
         <v>279</v>
       </c>
       <c r="D11" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" hidden="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" t="s">
         <v>164</v>
       </c>
@@ -1498,10 +1608,10 @@
         <v>279</v>
       </c>
       <c r="D12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" hidden="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -1512,10 +1622,10 @@
         <v>279</v>
       </c>
       <c r="D13" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" hidden="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -1526,10 +1636,10 @@
         <v>279</v>
       </c>
       <c r="D14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -1540,10 +1650,10 @@
         <v>279</v>
       </c>
       <c r="D15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" hidden="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -1554,7 +1664,7 @@
         <v>279</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:4" hidden="1">
@@ -1568,7 +1678,7 @@
         <v>279</v>
       </c>
       <c r="D17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:4" hidden="1">
@@ -1582,7 +1692,7 @@
         <v>279</v>
       </c>
       <c r="D18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:4" hidden="1">
@@ -1596,7 +1706,7 @@
         <v>279</v>
       </c>
       <c r="D19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:4" hidden="1">
@@ -1610,7 +1720,7 @@
         <v>279</v>
       </c>
       <c r="D20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:4" hidden="1">
@@ -1624,7 +1734,7 @@
         <v>279</v>
       </c>
       <c r="D21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:4" hidden="1">
@@ -1638,7 +1748,7 @@
         <v>279</v>
       </c>
       <c r="D22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1">
@@ -1652,7 +1762,7 @@
         <v>279</v>
       </c>
       <c r="D23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1">
@@ -1666,7 +1776,7 @@
         <v>279</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1">
@@ -1680,7 +1790,7 @@
         <v>279</v>
       </c>
       <c r="D25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:4" hidden="1">
@@ -1694,7 +1804,7 @@
         <v>279</v>
       </c>
       <c r="D26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1">
@@ -1708,7 +1818,7 @@
         <v>279</v>
       </c>
       <c r="D27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1">
@@ -1722,7 +1832,7 @@
         <v>279</v>
       </c>
       <c r="D28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1">
@@ -1736,7 +1846,7 @@
         <v>279</v>
       </c>
       <c r="D29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1">
@@ -1750,7 +1860,7 @@
         <v>279</v>
       </c>
       <c r="D30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:4" hidden="1">
@@ -1764,7 +1874,7 @@
         <v>279</v>
       </c>
       <c r="D31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:4" hidden="1">
@@ -1778,7 +1888,7 @@
         <v>279</v>
       </c>
       <c r="D32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:4" hidden="1">
@@ -1792,7 +1902,7 @@
         <v>279</v>
       </c>
       <c r="D33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:4" hidden="1">
@@ -1806,7 +1916,7 @@
         <v>279</v>
       </c>
       <c r="D34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1">
@@ -1820,7 +1930,7 @@
         <v>279</v>
       </c>
       <c r="D35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1">
@@ -1834,7 +1944,7 @@
         <v>279</v>
       </c>
       <c r="D36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:4" hidden="1">
@@ -1848,7 +1958,7 @@
         <v>279</v>
       </c>
       <c r="D37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:4" hidden="1">
@@ -1862,7 +1972,7 @@
         <v>279</v>
       </c>
       <c r="D38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:4" hidden="1">
@@ -1876,7 +1986,7 @@
         <v>279</v>
       </c>
       <c r="D39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:4" hidden="1">
@@ -1890,7 +2000,7 @@
         <v>279</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:4" hidden="1">
@@ -1904,7 +2014,7 @@
         <v>279</v>
       </c>
       <c r="D41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:4" hidden="1">
@@ -1918,7 +2028,7 @@
         <v>279</v>
       </c>
       <c r="D42" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="43" spans="1:4" hidden="1">
@@ -1932,7 +2042,7 @@
         <v>279</v>
       </c>
       <c r="D43" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:4" hidden="1">
@@ -1946,7 +2056,7 @@
         <v>279</v>
       </c>
       <c r="D44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="1:4" hidden="1">
@@ -1960,7 +2070,7 @@
         <v>279</v>
       </c>
       <c r="D45" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:4" hidden="1">
@@ -1974,7 +2084,7 @@
         <v>279</v>
       </c>
       <c r="D46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:4" hidden="1">
@@ -1988,7 +2098,7 @@
         <v>279</v>
       </c>
       <c r="D47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="1:4" hidden="1">
@@ -2002,7 +2112,7 @@
         <v>279</v>
       </c>
       <c r="D48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1">
@@ -2016,7 +2126,7 @@
         <v>279</v>
       </c>
       <c r="D49" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:4" hidden="1">
@@ -2030,7 +2140,7 @@
         <v>279</v>
       </c>
       <c r="D50" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="51" spans="1:4" hidden="1">
@@ -2044,7 +2154,7 @@
         <v>279</v>
       </c>
       <c r="D51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:4" hidden="1">
@@ -2058,7 +2168,7 @@
         <v>279</v>
       </c>
       <c r="D52" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:4" hidden="1">
@@ -2072,7 +2182,7 @@
         <v>279</v>
       </c>
       <c r="D53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:4" hidden="1">
@@ -2086,7 +2196,7 @@
         <v>279</v>
       </c>
       <c r="D54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1">
@@ -2100,7 +2210,7 @@
         <v>279</v>
       </c>
       <c r="D55" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="1:4" hidden="1">
@@ -2114,7 +2224,7 @@
         <v>279</v>
       </c>
       <c r="D56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:4" hidden="1">
@@ -2128,7 +2238,7 @@
         <v>279</v>
       </c>
       <c r="D57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:4" hidden="1">
@@ -2142,7 +2252,7 @@
         <v>279</v>
       </c>
       <c r="D58" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:4" hidden="1">
@@ -2156,7 +2266,7 @@
         <v>279</v>
       </c>
       <c r="D59" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:4" hidden="1">
@@ -2170,7 +2280,7 @@
         <v>279</v>
       </c>
       <c r="D60" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:4" hidden="1">
@@ -2184,7 +2294,7 @@
         <v>279</v>
       </c>
       <c r="D61" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:4" hidden="1">
@@ -2198,7 +2308,7 @@
         <v>279</v>
       </c>
       <c r="D62" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" spans="1:4" hidden="1">
@@ -2212,7 +2322,7 @@
         <v>279</v>
       </c>
       <c r="D63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="64" spans="1:4" hidden="1">
@@ -2226,7 +2336,7 @@
         <v>279</v>
       </c>
       <c r="D64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:4" hidden="1">
@@ -2240,7 +2350,7 @@
         <v>279</v>
       </c>
       <c r="D65" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:4" hidden="1">
@@ -2254,7 +2364,7 @@
         <v>279</v>
       </c>
       <c r="D66" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:4" hidden="1">
@@ -2268,7 +2378,7 @@
         <v>279</v>
       </c>
       <c r="D67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:4" hidden="1">
@@ -2282,7 +2392,7 @@
         <v>279</v>
       </c>
       <c r="D68" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="69" spans="1:4" hidden="1">
@@ -2296,7 +2406,7 @@
         <v>279</v>
       </c>
       <c r="D69" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="70" spans="1:4" hidden="1">
@@ -2310,7 +2420,7 @@
         <v>279</v>
       </c>
       <c r="D70" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="71" spans="1:4" hidden="1">
@@ -2324,7 +2434,7 @@
         <v>279</v>
       </c>
       <c r="D71" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:4" hidden="1">
@@ -2338,7 +2448,7 @@
         <v>279</v>
       </c>
       <c r="D72" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:4" hidden="1">
@@ -2352,7 +2462,7 @@
         <v>279</v>
       </c>
       <c r="D73" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="74" spans="1:4" hidden="1">
@@ -2366,7 +2476,7 @@
         <v>279</v>
       </c>
       <c r="D74" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="75" spans="1:4" hidden="1">
@@ -2380,7 +2490,7 @@
         <v>279</v>
       </c>
       <c r="D75" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="76" spans="1:4" hidden="1">
@@ -2394,7 +2504,7 @@
         <v>279</v>
       </c>
       <c r="D76" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="77" spans="1:4" hidden="1">
@@ -2408,7 +2518,7 @@
         <v>279</v>
       </c>
       <c r="D77" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="78" spans="1:4" hidden="1">
@@ -2422,7 +2532,7 @@
         <v>279</v>
       </c>
       <c r="D78" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="79" spans="1:4" hidden="1">
@@ -2436,7 +2546,7 @@
         <v>279</v>
       </c>
       <c r="D79" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="80" spans="1:4" hidden="1">
@@ -2450,7 +2560,7 @@
         <v>279</v>
       </c>
       <c r="D80" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:4" hidden="1">
@@ -2464,7 +2574,7 @@
         <v>279</v>
       </c>
       <c r="D81" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:4" hidden="1">
@@ -2478,7 +2588,7 @@
         <v>279</v>
       </c>
       <c r="D82" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:4" hidden="1">
@@ -2492,7 +2602,7 @@
         <v>279</v>
       </c>
       <c r="D83" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1">
@@ -2506,7 +2616,7 @@
         <v>279</v>
       </c>
       <c r="D84" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="85" spans="1:4" hidden="1">
@@ -2520,7 +2630,7 @@
         <v>279</v>
       </c>
       <c r="D85" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="86" spans="1:4" hidden="1">
@@ -2534,7 +2644,7 @@
         <v>279</v>
       </c>
       <c r="D86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:4" hidden="1">
@@ -2548,7 +2658,7 @@
         <v>279</v>
       </c>
       <c r="D87" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="88" spans="1:4" hidden="1">
@@ -2562,7 +2672,7 @@
         <v>279</v>
       </c>
       <c r="D88" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="89" spans="1:4" hidden="1">
@@ -2576,7 +2686,7 @@
         <v>279</v>
       </c>
       <c r="D89" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:4" hidden="1">
@@ -2590,7 +2700,7 @@
         <v>279</v>
       </c>
       <c r="D90" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:4" hidden="1">
@@ -2604,7 +2714,7 @@
         <v>279</v>
       </c>
       <c r="D91" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:4" hidden="1">
@@ -2618,7 +2728,7 @@
         <v>279</v>
       </c>
       <c r="D92" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:4" hidden="1">
@@ -2632,7 +2742,7 @@
         <v>279</v>
       </c>
       <c r="D93" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:4" hidden="1">
@@ -2646,7 +2756,7 @@
         <v>279</v>
       </c>
       <c r="D94" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:4" hidden="1">
@@ -2660,7 +2770,7 @@
         <v>279</v>
       </c>
       <c r="D95" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="96" spans="1:4" hidden="1">
@@ -2674,7 +2784,7 @@
         <v>279</v>
       </c>
       <c r="D96" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="97" spans="1:4" hidden="1">
@@ -2688,7 +2798,7 @@
         <v>279</v>
       </c>
       <c r="D97" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:4" hidden="1">
@@ -2702,7 +2812,7 @@
         <v>279</v>
       </c>
       <c r="D98" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="1:4" hidden="1">
@@ -2716,7 +2826,7 @@
         <v>279</v>
       </c>
       <c r="D99" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="1:4" hidden="1">
@@ -2730,7 +2840,7 @@
         <v>279</v>
       </c>
       <c r="D100" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:4" hidden="1">
@@ -2744,7 +2854,7 @@
         <v>279</v>
       </c>
       <c r="D101" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="102" spans="1:4" hidden="1">
@@ -2758,7 +2868,7 @@
         <v>279</v>
       </c>
       <c r="D102" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="103" spans="1:4" hidden="1">
@@ -2772,7 +2882,7 @@
         <v>279</v>
       </c>
       <c r="D103" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:4" hidden="1">
@@ -2786,7 +2896,7 @@
         <v>279</v>
       </c>
       <c r="D104" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:4" hidden="1">
@@ -2800,7 +2910,7 @@
         <v>279</v>
       </c>
       <c r="D105" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:4" hidden="1">
@@ -2814,7 +2924,7 @@
         <v>279</v>
       </c>
       <c r="D106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:4" hidden="1">
@@ -2828,7 +2938,7 @@
         <v>279</v>
       </c>
       <c r="D107" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="1:4" hidden="1">
@@ -2842,7 +2952,7 @@
         <v>279</v>
       </c>
       <c r="D108" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" spans="1:4" hidden="1">
@@ -4110,7 +4220,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" hidden="1">
       <c r="A224" t="s">
         <v>1</v>
       </c>
@@ -4118,10 +4228,10 @@
         <v>46</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" hidden="1">
       <c r="A225" t="s">
         <v>1</v>
       </c>
@@ -4129,10 +4239,10 @@
         <v>45</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" hidden="1">
       <c r="A226" t="s">
         <v>1</v>
       </c>
@@ -4140,10 +4250,10 @@
         <v>44</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" hidden="1">
       <c r="A227" t="s">
         <v>1</v>
       </c>
@@ -4151,10 +4261,10 @@
         <v>43</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" hidden="1">
       <c r="A228" t="s">
         <v>1</v>
       </c>
@@ -4162,10 +4272,10 @@
         <v>42</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" hidden="1">
       <c r="A229" t="s">
         <v>1</v>
       </c>
@@ -4173,10 +4283,10 @@
         <v>41</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" hidden="1">
       <c r="A230" t="s">
         <v>1</v>
       </c>
@@ -4184,10 +4294,10 @@
         <v>40</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" hidden="1">
       <c r="A231" t="s">
         <v>1</v>
       </c>
@@ -4195,10 +4305,10 @@
         <v>39</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" hidden="1">
       <c r="A232" t="s">
         <v>1</v>
       </c>
@@ -4206,10 +4316,10 @@
         <v>38</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" hidden="1">
       <c r="A233" t="s">
         <v>1</v>
       </c>
@@ -4217,10 +4327,10 @@
         <v>37</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" hidden="1">
       <c r="A234" t="s">
         <v>1</v>
       </c>
@@ -4228,10 +4338,10 @@
         <v>36</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" hidden="1">
       <c r="A235" t="s">
         <v>1</v>
       </c>
@@ -4239,10 +4349,10 @@
         <v>35</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" hidden="1">
       <c r="A236" t="s">
         <v>1</v>
       </c>
@@ -4250,10 +4360,10 @@
         <v>34</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" hidden="1">
       <c r="A237" t="s">
         <v>1</v>
       </c>
@@ -4261,10 +4371,10 @@
         <v>33</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" hidden="1">
       <c r="A238" t="s">
         <v>1</v>
       </c>
@@ -4272,10 +4382,10 @@
         <v>32</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" hidden="1">
       <c r="A239" t="s">
         <v>1</v>
       </c>
@@ -4283,10 +4393,10 @@
         <v>31</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" hidden="1">
       <c r="A240" t="s">
         <v>1</v>
       </c>
@@ -4294,10 +4404,10 @@
         <v>30</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" hidden="1">
       <c r="A241" t="s">
         <v>1</v>
       </c>
@@ -4305,10 +4415,10 @@
         <v>29</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" hidden="1">
       <c r="A242" t="s">
         <v>1</v>
       </c>
@@ -4316,10 +4426,10 @@
         <v>28</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" hidden="1">
       <c r="A243" t="s">
         <v>1</v>
       </c>
@@ -4327,10 +4437,10 @@
         <v>27</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" hidden="1">
       <c r="A244" t="s">
         <v>1</v>
       </c>
@@ -4338,10 +4448,10 @@
         <v>26</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" hidden="1">
       <c r="A245" t="s">
         <v>1</v>
       </c>
@@ -4349,10 +4459,10 @@
         <v>25</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" hidden="1">
       <c r="A246" t="s">
         <v>1</v>
       </c>
@@ -4360,10 +4470,10 @@
         <v>24</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" hidden="1">
       <c r="A247" t="s">
         <v>1</v>
       </c>
@@ -4371,10 +4481,10 @@
         <v>23</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" hidden="1">
       <c r="A248" t="s">
         <v>1</v>
       </c>
@@ -4382,10 +4492,10 @@
         <v>22</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" hidden="1">
       <c r="A249" t="s">
         <v>1</v>
       </c>
@@ -4393,10 +4503,10 @@
         <v>21</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" hidden="1">
       <c r="A250" t="s">
         <v>1</v>
       </c>
@@ -4404,10 +4514,10 @@
         <v>20</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" hidden="1">
       <c r="A251" t="s">
         <v>1</v>
       </c>
@@ -4415,10 +4525,10 @@
         <v>19</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" hidden="1">
       <c r="A252" t="s">
         <v>1</v>
       </c>
@@ -4426,10 +4536,10 @@
         <v>18</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" hidden="1">
       <c r="A253" t="s">
         <v>1</v>
       </c>
@@ -4437,10 +4547,10 @@
         <v>17</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" hidden="1">
       <c r="A254" t="s">
         <v>1</v>
       </c>
@@ -4448,10 +4558,10 @@
         <v>16</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" hidden="1">
       <c r="A255" t="s">
         <v>1</v>
       </c>
@@ -4459,10 +4569,10 @@
         <v>15</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" hidden="1">
       <c r="A256" t="s">
         <v>1</v>
       </c>
@@ -4470,10 +4580,10 @@
         <v>14</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" hidden="1">
       <c r="A257" t="s">
         <v>1</v>
       </c>
@@ -4481,10 +4591,10 @@
         <v>13</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" hidden="1">
       <c r="A258" t="s">
         <v>1</v>
       </c>
@@ -4492,10 +4602,10 @@
         <v>12</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" hidden="1">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -4503,10 +4613,10 @@
         <v>11</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" hidden="1">
       <c r="A260" t="s">
         <v>1</v>
       </c>
@@ -4514,10 +4624,10 @@
         <v>10</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" hidden="1">
       <c r="A261" t="s">
         <v>1</v>
       </c>
@@ -4525,10 +4635,10 @@
         <v>9</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" hidden="1">
       <c r="A262" t="s">
         <v>1</v>
       </c>
@@ -4536,10 +4646,10 @@
         <v>8</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" hidden="1">
       <c r="A263" t="s">
         <v>1</v>
       </c>
@@ -4547,10 +4657,10 @@
         <v>7</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" hidden="1">
       <c r="A264" t="s">
         <v>1</v>
       </c>
@@ -4558,10 +4668,10 @@
         <v>6</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" hidden="1">
       <c r="A265" t="s">
         <v>1</v>
       </c>
@@ -4569,10 +4679,10 @@
         <v>5</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" hidden="1">
       <c r="A266" t="s">
         <v>1</v>
       </c>
@@ -4580,10 +4690,10 @@
         <v>4</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" hidden="1">
       <c r="A267" t="s">
         <v>1</v>
       </c>
@@ -4591,10 +4701,10 @@
         <v>3</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" hidden="1">
       <c r="A268" t="s">
         <v>1</v>
       </c>
@@ -4602,10 +4712,10 @@
         <v>2</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" hidden="1">
       <c r="A269" t="s">
         <v>1</v>
       </c>
@@ -4613,14 +4723,14 @@
         <v>0</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D269">
     <filterColumn colId="0">
       <filters>
-        <filter val="molluscs"/>
+        <filter val="crustacea_arthropods"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4630,6 +4740,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated representativeness spreadsheet based on Mike Kingsford input
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/spp_gp_representativeness.xlsx
+++ b/_raw_data/xlsx/spp_gp_representativeness.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12200" yWindow="380" windowWidth="20500" windowHeight="13480" tabRatio="500"/>
+    <workbookView xWindow="12200" yWindow="380" windowWidth="20500" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="215">
   <si>
     <t>turbo militaris</t>
   </si>
@@ -635,13 +635,82 @@
   </si>
   <si>
     <t>comments/notes</t>
+  </si>
+  <si>
+    <t>Acanthopagrus australis</t>
+  </si>
+  <si>
+    <t>Amphiprion akindynos</t>
+  </si>
+  <si>
+    <t>Brachionichthys hirsutus</t>
+  </si>
+  <si>
+    <t>Cephalopholis cyanostigmata</t>
+  </si>
+  <si>
+    <t>Clupea harengus</t>
+  </si>
+  <si>
+    <t>Corphaena hippurus</t>
+  </si>
+  <si>
+    <t>Chromis atripectoralis</t>
+  </si>
+  <si>
+    <t>Chromis dispilus</t>
+  </si>
+  <si>
+    <t>Engraulis ringens</t>
+  </si>
+  <si>
+    <t>Epinephelus coioides</t>
+  </si>
+  <si>
+    <t>Epinephelus fasciatus</t>
+  </si>
+  <si>
+    <t>Hoplostethus japonicus</t>
+  </si>
+  <si>
+    <t>Molva dypterygia</t>
+  </si>
+  <si>
+    <t>Oncorhynchus nerka</t>
+  </si>
+  <si>
+    <t>Pagrus auratus</t>
+  </si>
+  <si>
+    <t>Pomacentrus amboinensis</t>
+  </si>
+  <si>
+    <t>Parma microlepis</t>
+  </si>
+  <si>
+    <t>Plectropomus leopardus</t>
+  </si>
+  <si>
+    <t>Plectropomus areolatus</t>
+  </si>
+  <si>
+    <t>Rexea solandri</t>
+  </si>
+  <si>
+    <t>Spratelloides delicatulus</t>
+  </si>
+  <si>
+    <t>Thunnus maccoyii</t>
+  </si>
+  <si>
+    <t>fish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,13 +755,48 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -709,12 +813,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1061,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109:XFD223"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155:C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3002,7 +3128,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>1</v>
       </c>
@@ -3013,7 +3139,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>1</v>
       </c>
@@ -3024,7 +3150,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>1</v>
       </c>
@@ -3035,7 +3161,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>1</v>
       </c>
@@ -3046,7 +3172,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>1</v>
       </c>
@@ -3057,7 +3183,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>1</v>
       </c>
@@ -3068,7 +3194,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -3079,7 +3205,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3216,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>1</v>
       </c>
@@ -3101,7 +3227,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -3110,6 +3236,314 @@
       </c>
       <c r="C154" s="1" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>214</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D155" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>214</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D156" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>214</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D157" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>214</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D158" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>214</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D159" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>214</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D160" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>214</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C161" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D161" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="s">
+        <v>214</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D162" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>214</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C163" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D163" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>214</v>
+      </c>
+      <c r="B164" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D164" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>214</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C165" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D165" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>214</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D166" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>214</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C167" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D167" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>214</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C168" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D168" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>214</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C169" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D169" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="s">
+        <v>214</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D170" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="s">
+        <v>214</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D171" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>214</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D172" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>214</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C173" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D173" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>214</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D174" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>214</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D175" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>214</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C176" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D176" s="5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fish traits (expanded Engraulis ringens to various genera) from Mike Kingsford
Former-commit-id: 484a208b83b824c2ee3409feabf3380d1044c74f
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/spp_gp_representativeness.xlsx
+++ b/_raw_data/xlsx/spp_gp_representativeness.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="216">
   <si>
     <t>turbo militaris</t>
   </si>
@@ -704,6 +704,9 @@
   </si>
   <si>
     <t>fish</t>
+  </si>
+  <si>
+    <t>Meuschenia scaber</t>
   </si>
 </sst>
 </file>
@@ -1187,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F176"/>
+  <dimension ref="A1:F177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155:C176"/>
+      <selection activeCell="A177" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3544,6 +3547,20 @@
       </c>
       <c r="D176" s="5">
         <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
+        <v>214</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D177" s="5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>